<commit_message>
feat: error_code file generation.
</commit_message>
<xml_diff>
--- a/src/main/resources/error_code_template.xlsx
+++ b/src/main/resources/error_code_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\error-code-demo\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\source\error-code-demo\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E9E8F9-D2F3-4FA9-B3D3-A9EC06E2643F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A80D844-D537-451E-93E1-49D3D0C52DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>课题系统所有错误信息整理</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>分类</t>
   </si>
@@ -86,45 +72,7 @@
     <t>获取数据失败</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>方法|实体类</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LACK_OF_PARAMS</t>
-  </si>
-  <si>
-    <t>ERROR_CODE_00002</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>缺少参数</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>业务部分</t>
-  </si>
-  <si>
-    <t>ERROR_CODE_00100</t>
-  </si>
-  <si>
-    <t>ERROR_CODE_00200</t>
   </si>
   <si>
     <t>实体类</t>
@@ -134,43 +82,50 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>USERNAME_CAN_NOT_BE_REPEATED</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR_CODE_00100</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR_CODE_00200</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ROLE_NOT_EXIST</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色不存在</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XX系统错误信息</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户名不可以重复</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>USERNAME_CAN_NOT_BE_BLANK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR_CODE_00101</t>
+  </si>
+  <si>
+    <t>用户名不能为空</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>User-用户错误信息</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>Role-角色错误信息</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>User-用户错误信息</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>USERNAME_CAN_NOT_BE_BLANK</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PASSWORD_CAN_NOT_BE_BLANK</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户名不能为空</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>密码不能为空</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>角色ID不能重复</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ROLE_ID_CAN_NOT_REPEAT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>USERNAME_CAN_NOT_REPEAT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户名不能重复</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -178,7 +133,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,12 +159,6 @@
     <font>
       <sz val="24"/>
       <color rgb="FF000000"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="微软雅黑"/>
       <family val="2"/>
       <charset val="134"/>
@@ -261,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -284,41 +233,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -601,7 +595,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
@@ -614,170 +608,142 @@
   <cols>
     <col min="2" max="2" width="33.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.75" customWidth="1"/>
+    <col min="4" max="4" width="38.375" customWidth="1"/>
     <col min="5" max="5" width="18.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.375" customWidth="1"/>
+    <col min="6" max="6" width="20.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="40.5" customHeight="1">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="A1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" ht="16.5">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5">
-      <c r="A4" s="9"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="C5" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5">
-      <c r="A6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11" t="s">
-        <v>26</v>
+      <c r="A7" s="11"/>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16.5">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16.5">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B6"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1" promptTitle="提示" prompt="您选择的不是下拉列表中的选项" sqref="C3:C9" xr:uid="{A3C128F7-82D8-4007-92F3-F1D2DE46A81C}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1" promptTitle="提示" prompt="您选择的不是下拉列表中的选项" sqref="C3:C7" xr:uid="{A3C128F7-82D8-4007-92F3-F1D2DE46A81C}">
       <formula1>"方法,实体类,方法|实体类"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>